<commit_message>
segundo bac (solo los nombres)
</commit_message>
<xml_diff>
--- a/HT-4/Optica BAC-01-Catálogo de actores.xlsx
+++ b/HT-4/Optica BAC-01-Catálogo de actores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6474FB-F705-064E-8BEF-9A8D01BAFC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E5155B-A590-A147-B81C-48F226AA3E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Nombre</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>No sé si llamarlos así lol</t>
+  </si>
+  <si>
+    <t>Comprador</t>
+  </si>
+  <si>
+    <t>Persona que desea adquirir una montura nueva o unos lentes o reparar sus lentes o montura o requiere de un examen visual</t>
+  </si>
+  <si>
+    <t>&gt; Esto es en caso de que sea solo con un cliente (que no creo)</t>
   </si>
 </sst>
 </file>
@@ -132,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -164,11 +173,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -181,10 +199,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -501,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -512,25 +533,25 @@
     <col min="3" max="3" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
@@ -541,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -552,7 +573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -563,7 +584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
@@ -574,7 +595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -585,32 +606,57 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="90" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>